<commit_message>
compression des images avec compressor.io
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VnZnX\Desktop\Info\P4_Galpin_Vincent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC32DC0D-E628-482E-88D2-A5852EC56073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06934863-15A9-47DD-A367-23B315BAF93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>Catégorie</t>
   </si>
@@ -284,6 +284,15 @@
   </si>
   <si>
     <t>Au clic de l'internaute sur l'adresse de l'entreprise ouvre google map à la bonne adresse</t>
+  </si>
+  <si>
+    <t>Navigation clavier</t>
+  </si>
+  <si>
+    <t>Ajouter une navigation grace au clavier avec Tab et Maj + Tab</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6941406-rendez-les-interactions-sur-le-site-accessibles</t>
   </si>
 </sst>
 </file>
@@ -365,7 +374,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -432,13 +441,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -455,23 +473,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -483,7 +495,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -705,7 +729,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -715,7 +739,7 @@
     <col min="3" max="3" width="38.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="73.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="98.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="113.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -759,9 +783,9 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:26" s="8" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
@@ -781,7 +805,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
+      <c r="A4" s="11"/>
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -799,7 +823,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
@@ -817,7 +841,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
@@ -827,7 +851,7 @@
       <c r="D6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -835,7 +859,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
@@ -845,13 +869,13 @@
       <c r="D7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="3" t="s">
         <v>35</v>
       </c>
@@ -869,7 +893,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="3" t="s">
         <v>40</v>
       </c>
@@ -879,15 +903,15 @@
       <c r="D9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="17" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="3" t="s">
         <v>45</v>
       </c>
@@ -897,11 +921,11 @@
       <c r="D10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="3" t="s">
         <v>47</v>
       </c>
@@ -919,7 +943,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
@@ -946,7 +970,7 @@
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -964,7 +988,7 @@
       </c>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
@@ -980,7 +1004,7 @@
       </c>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="3" t="s">
         <v>63</v>
       </c>
@@ -996,7 +1020,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="3" t="s">
         <v>65</v>
       </c>
@@ -1012,92 +1036,103 @@
       </c>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+      <c r="A20" s="11"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:26" s="13" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="15"/>
-      <c r="Z21" s="16"/>
+    <row r="21" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="14"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
       <c r="F23" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="12"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="9" t="s">
         <v>79</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E26" s="6"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E27" s="6"/>
@@ -2085,13 +2120,14 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="A22:A26"/>
     <mergeCell ref="A2:XFD2"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A22:A25"/>
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="A21:XFD21"/>
     <mergeCell ref="E6:E7"/>
@@ -2115,8 +2151,9 @@
     <hyperlink ref="F18" r:id="rId13" xr:uid="{BA75C060-509A-413A-B248-E2454E726CD9}"/>
     <hyperlink ref="F22" r:id="rId14" xr:uid="{719BD7BF-D2F8-4D58-A319-26855C3A3F58}"/>
     <hyperlink ref="F23" r:id="rId15" location="cr%C3%A9er_un_lien_avec_une_adresse_%C3%A9lectronique" xr:uid="{62CCAFD2-EDC0-446D-9B2B-DDE61F25C012}"/>
+    <hyperlink ref="F26" r:id="rId16" xr:uid="{5B1DC9AF-62E5-4373-BA39-20C4C7FE55AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId16"/>
+  <pageSetup orientation="landscape" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>